<commit_message>
Creating registration tests, and adding loggs.
</commit_message>
<xml_diff>
--- a/src/test/resources/testData.xlsx
+++ b/src/test/resources/testData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CP24\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CP24\selenium_opencart_abstracta_us\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38797504-15B1-4E3D-AD5C-65D909B9B415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6687C779-129F-42F0-84C6-D38337516D4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>FirstName</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>t@t.com</t>
+  </si>
+  <si>
+    <t>T123123123</t>
   </si>
 </sst>
 </file>
@@ -99,9 +102,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperłącze" xfId="1" builtinId="8"/>
@@ -386,12 +390,12 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
@@ -404,7 +408,7 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -418,8 +422,8 @@
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2">
-        <v>123123123</v>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
@@ -432,8 +436,8 @@
       <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3">
-        <v>123123123</v>
+      <c r="D3" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -442,5 +446,6 @@
     <hyperlink ref="C3" r:id="rId2" xr:uid="{3D678366-2893-439C-BF56-60CC4BED7C6C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>